<commit_message>
Login has been created. Messages for log in still need to be added some css, they can't be seen since they are overlapped with the navbar
</commit_message>
<xml_diff>
--- a/Req.xlsx
+++ b/Req.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ypini\Desktop\urbanohome\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{56B4C85A-6928-4004-92E4-383D8FA7E3A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D20E76C-5897-4569-B5E4-62A91D683C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{8D819641-AC54-4F9D-8D24-2392321D3152}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8D819641-AC54-4F9D-8D24-2392321D3152}"/>
   </bookViews>
   <sheets>
     <sheet name="Funcionales" sheetId="1" r:id="rId1"/>
@@ -351,7 +351,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -382,6 +382,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -530,7 +536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -541,6 +547,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -550,48 +598,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -906,10 +913,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{147DD500-7CDC-4014-9AE1-1DA1A5ACD366}">
-  <dimension ref="B1:E50"/>
+  <dimension ref="B1:F50"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,298 +925,299 @@
     <col min="4" max="4" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+      <c r="E2" s="20"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+    <row r="4" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="9" t="s">
+      <c r="F4" s="21"/>
+    </row>
+    <row r="5" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
+    <row r="6" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
+    <row r="7" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
+    <row r="8" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="s">
+    <row r="9" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
+    <row r="10" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B11" s="9" t="s">
+    <row r="11" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B12" s="9" t="s">
+    <row r="12" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="9" t="s">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="9" t="s">
+    <row r="14" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B15" s="9" t="s">
+    <row r="15" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="9" t="s">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="9" t="s">
+    <row r="17" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E17" s="17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B18" s="9" t="s">
+    <row r="18" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B19" s="9" t="s">
+    <row r="19" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E19" s="17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="9" t="s">
+    <row r="20" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E20" s="17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B21" s="9" t="s">
+    <row r="21" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E21" s="17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="2:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="10" t="s">
+    <row r="22" spans="2:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="E22" s="16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>72</v>
       </c>
@@ -1222,56 +1230,57 @@
       <c r="E23" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="21"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1398,7 +1407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1324D62D-D555-408B-A357-6151F7F77940}">
   <dimension ref="B4:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -1410,226 +1419,226 @@
   <sheetData>
     <row r="4" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="19"/>
+      <c r="D5" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="6"/>
+      <c r="E5" s="20"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="15" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="15" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="15" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="E10" s="18"/>
+      <c r="E10" s="15"/>
     </row>
     <row r="11" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="E11" s="18"/>
+      <c r="E11" s="15"/>
     </row>
     <row r="12" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="E12" s="18"/>
+      <c r="E12" s="15"/>
     </row>
     <row r="13" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="E13" s="18"/>
+      <c r="E13" s="15"/>
     </row>
     <row r="14" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="E14" s="18"/>
+      <c r="E14" s="15"/>
     </row>
     <row r="15" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="E15" s="18"/>
+      <c r="E15" s="15"/>
     </row>
     <row r="16" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="E16" s="18"/>
+      <c r="E16" s="15"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="20"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="17"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="20"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="17"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="18"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="15"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="20"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="17"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="20"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="17"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="20"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="17"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="20"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="17"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="20"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="17"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="19"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
navbar has been updated to show username when logged in and show logout. Logout option working.
</commit_message>
<xml_diff>
--- a/Req.xlsx
+++ b/Req.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ypini\Desktop\urbanohome\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D20E76C-5897-4569-B5E4-62A91D683C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11F9A3F-46ED-49AE-89C6-222B74E53CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8D819641-AC54-4F9D-8D24-2392321D3152}"/>
   </bookViews>
@@ -589,6 +589,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -598,7 +599,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -916,7 +916,7 @@
   <dimension ref="B1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,14 +927,14 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="20"/>
+      <c r="E2" s="21"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
@@ -963,7 +963,7 @@
       <c r="E4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="21"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -978,6 +978,7 @@
       <c r="E5" s="15" t="s">
         <v>15</v>
       </c>
+      <c r="F5" s="18"/>
     </row>
     <row r="6" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
@@ -1230,7 +1231,7 @@
       <c r="E23" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F23" s="21"/>
+      <c r="F23" s="18"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
@@ -1419,14 +1420,14 @@
   <sheetData>
     <row r="4" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19" t="s">
+      <c r="C5" s="20"/>
+      <c r="D5" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="20"/>
+      <c r="E5" s="21"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">

</xml_diff>

<commit_message>
Product grid has been updated
</commit_message>
<xml_diff>
--- a/Req.xlsx
+++ b/Req.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ypini\Desktop\urbanohome\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11F9A3F-46ED-49AE-89C6-222B74E53CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538652C1-FE6C-4EF2-A080-2B95D69C16F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8D819641-AC54-4F9D-8D24-2392321D3152}"/>
   </bookViews>
@@ -916,7 +916,7 @@
   <dimension ref="B1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,6 +993,7 @@
       <c r="E6" s="15" t="s">
         <v>15</v>
       </c>
+      <c r="F6" s="18"/>
     </row>
     <row r="7" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
@@ -1147,6 +1148,7 @@
       <c r="E17" s="17" t="s">
         <v>40</v>
       </c>
+      <c r="F17" s="18"/>
     </row>
     <row r="18" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
@@ -1161,6 +1163,7 @@
       <c r="E18" s="17" t="s">
         <v>40</v>
       </c>
+      <c r="F18" s="18"/>
     </row>
     <row r="19" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
@@ -1175,6 +1178,7 @@
       <c r="E19" s="17" t="s">
         <v>40</v>
       </c>
+      <c r="F19" s="18"/>
     </row>
     <row r="20" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
@@ -1189,6 +1193,7 @@
       <c r="E20" s="17" t="s">
         <v>40</v>
       </c>
+      <c r="F20" s="18"/>
     </row>
     <row r="21" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">

</xml_diff>

<commit_message>
Excel has been updated
</commit_message>
<xml_diff>
--- a/Req.xlsx
+++ b/Req.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ypini\Desktop\urbanohome\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538652C1-FE6C-4EF2-A080-2B95D69C16F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334C52A0-1FCF-48C5-B104-69C57C8862F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8D819641-AC54-4F9D-8D24-2392321D3152}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="91">
   <si>
     <t>Requerimientos</t>
   </si>
@@ -336,6 +336,9 @@
   <si>
     <t xml:space="preserve">Al realizar una compra (venta), el carrito de
 compras se reinicia </t>
+  </si>
+  <si>
+    <t>Se puede hacer al agregar el producto por primera vez, pero una vez añadido aún no se puede modificar</t>
   </si>
 </sst>
 </file>
@@ -351,7 +354,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -388,6 +391,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -536,7 +545,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -599,6 +608,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -913,10 +923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{147DD500-7CDC-4014-9AE1-1DA1A5ACD366}">
-  <dimension ref="B1:F50"/>
+  <dimension ref="B1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,8 +935,8 @@
     <col min="4" max="4" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
@@ -936,7 +946,7 @@
       </c>
       <c r="E2" s="21"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
@@ -950,7 +960,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
@@ -965,7 +975,7 @@
       </c>
       <c r="F4" s="18"/>
     </row>
-    <row r="5" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
@@ -980,7 +990,7 @@
       </c>
       <c r="F5" s="18"/>
     </row>
-    <row r="6" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>11</v>
       </c>
@@ -995,7 +1005,7 @@
       </c>
       <c r="F6" s="18"/>
     </row>
-    <row r="7" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>16</v>
       </c>
@@ -1008,8 +1018,9 @@
       <c r="E7" s="15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="F7" s="18"/>
+    </row>
+    <row r="8" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>19</v>
       </c>
@@ -1022,8 +1033,12 @@
       <c r="E8" s="15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="F8" s="22"/>
+      <c r="G8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>22</v>
       </c>
@@ -1037,7 +1052,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>25</v>
       </c>
@@ -1051,7 +1066,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>28</v>
       </c>
@@ -1065,7 +1080,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>30</v>
       </c>
@@ -1079,7 +1094,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>34</v>
       </c>
@@ -1093,7 +1108,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
         <v>37</v>
       </c>
@@ -1107,7 +1122,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
         <v>41</v>
       </c>
@@ -1121,7 +1136,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
guardado button has been added, it is disabled by default, but when the user modifies the quantity, it gets enabled, and the text changes to guardar. Make guardar button an ajax request, and put disabled again is required
</commit_message>
<xml_diff>
--- a/Req.xlsx
+++ b/Req.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ypini\Desktop\urbanohome\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334C52A0-1FCF-48C5-B104-69C57C8862F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E6519D-9003-4142-9022-6E40AD768B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8D819641-AC54-4F9D-8D24-2392321D3152}"/>
   </bookViews>
@@ -354,7 +354,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -391,12 +391,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -545,7 +539,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -608,7 +602,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -925,8 +918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{147DD500-7CDC-4014-9AE1-1DA1A5ACD366}">
   <dimension ref="B1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,7 +1026,7 @@
       <c r="E8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="22"/>
+      <c r="F8" s="18"/>
       <c r="G8" t="s">
         <v>90</v>
       </c>

</xml_diff>

<commit_message>
sending function to ajax request has been converted into a function to save some lines. deletecart info has been created on the view. Is required now: create ajax request from cart settings on template, and delete product div that has been deleted on the db
</commit_message>
<xml_diff>
--- a/Req.xlsx
+++ b/Req.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ypini\Desktop\urbanohome\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E6519D-9003-4142-9022-6E40AD768B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3FAFE92-360E-40D6-9691-B678AC6C7A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8D819641-AC54-4F9D-8D24-2392321D3152}"/>
   </bookViews>
@@ -918,8 +918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{147DD500-7CDC-4014-9AE1-1DA1A5ACD366}">
   <dimension ref="B1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,6 +1044,7 @@
       <c r="E9" s="15" t="s">
         <v>15</v>
       </c>
+      <c r="F9" s="18"/>
     </row>
     <row r="10" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">

</xml_diff>